<commit_message>
Changes made in IAM for sanity
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Authoring.xlsx
+++ b/src/test/resources/xls/Authoring.xlsx
@@ -23,12 +23,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Test Cases'!$A$1:$E$71</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="269">
   <si>
     <t>TCID</t>
   </si>
@@ -813,13 +813,39 @@
   </si>
   <si>
     <t>Authoring9</t>
+  </si>
+  <si>
+    <t>Authoring71</t>
+  </si>
+  <si>
+    <t>Authoring72</t>
+  </si>
+  <si>
+    <t>Authoring73</t>
+  </si>
+  <si>
+    <t>Verify that user can see the flag option for post of other neon users</t>
+  </si>
+  <si>
+    <t>Verify that user is able to add links to the comment</t>
+  </si>
+  <si>
+    <t>Verify that the user is able to add external links to the post</t>
+  </si>
+  <si>
+    <t>Authoring74</t>
+  </si>
+  <si>
+    <t>OPQA-372</t>
+  </si>
+  <si>
+    <t>Verify that timestamp is associated with the user generated posts.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -948,7 +974,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -987,6 +1013,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1284,19 +1313,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75:E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="39.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="70.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="6.8046875" collapsed="true"/>
+    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="70.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="16" customFormat="1">
@@ -2505,6 +2534,66 @@
       <c r="E71" s="1" t="s">
         <v>28</v>
       </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="D72" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E72" s="1"/>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D73" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E73" s="1"/>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D74" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E74" s="1"/>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D75" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E75" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2574,8 +2663,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="56.0" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="56" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2628,11 +2717,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="55.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="43.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="55" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="43.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2691,9 +2780,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="28.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="58.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="1" max="1" width="28.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="58.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2809,10 +2898,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="45.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="83.5703125" collapsed="true"/>
-    <col min="4" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2850,12 +2939,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2917,11 +3006,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="70.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="47.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="70.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="47.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2980,10 +3069,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="54.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="11" customFormat="1">
@@ -3100,10 +3189,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="51.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="61.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="61.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3177,9 +3266,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="59.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="59.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3295,10 +3384,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="68.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="38.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="20.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="68.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="38" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3361,10 +3450,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="35.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="1" max="1" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="35.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>

<commit_message>
taking latest changes and adding java doc for profile test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Authoring.xlsx
+++ b/src/test/resources/xls/Authoring.xlsx
@@ -23,12 +23,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Test Cases'!$A$1:$E$71</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="269">
   <si>
     <t>TCID</t>
   </si>
@@ -813,13 +813,39 @@
   </si>
   <si>
     <t>Authoring9</t>
+  </si>
+  <si>
+    <t>Authoring71</t>
+  </si>
+  <si>
+    <t>Authoring72</t>
+  </si>
+  <si>
+    <t>Authoring73</t>
+  </si>
+  <si>
+    <t>Verify that user can see the flag option for post of other neon users</t>
+  </si>
+  <si>
+    <t>Verify that user is able to add links to the comment</t>
+  </si>
+  <si>
+    <t>Verify that the user is able to add external links to the post</t>
+  </si>
+  <si>
+    <t>Authoring74</t>
+  </si>
+  <si>
+    <t>OPQA-372</t>
+  </si>
+  <si>
+    <t>Verify that timestamp is associated with the user generated posts.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -948,7 +974,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -987,6 +1013,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1284,19 +1313,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75:E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="39.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="70.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="6.8046875" collapsed="true"/>
+    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="70.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="16" customFormat="1">
@@ -2505,6 +2534,66 @@
       <c r="E71" s="1" t="s">
         <v>28</v>
       </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="D72" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E72" s="1"/>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D73" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E73" s="1"/>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D74" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E74" s="1"/>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D75" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E75" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2574,8 +2663,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="56.0" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="56" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2628,11 +2717,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="55.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="43.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="55" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="43.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2691,9 +2780,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="28.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="58.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="1" max="1" width="28.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="58.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2809,10 +2898,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="45.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="83.5703125" collapsed="true"/>
-    <col min="4" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2850,12 +2939,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2917,11 +3006,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="70.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="47.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="70.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="47.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2980,10 +3069,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="54.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="11" customFormat="1">
@@ -3100,10 +3189,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="51.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="61.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="61.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3177,9 +3266,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="59.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="59.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3295,10 +3384,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="68.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="38.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="20.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="68.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="38" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3361,10 +3450,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="35.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="1" max="1" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="35.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>

<commit_message>
Merged the tests and updated the excel
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Authoring.xlsx
+++ b/src/test/resources/xls/Authoring.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="275">
   <si>
     <t>TCID</t>
   </si>
@@ -840,6 +840,24 @@
   </si>
   <si>
     <t>Verify that timestamp is associated with the user generated posts.</t>
+  </si>
+  <si>
+    <t>Authoring75</t>
+  </si>
+  <si>
+    <t>Authoring76</t>
+  </si>
+  <si>
+    <t>OPQA-1195|OPQA-1313|OPQA-1312|OPQA-1090|OPQA-1201</t>
+  </si>
+  <si>
+    <t>Verify saving post as draft, accessing it for edit from profile,delete post from prfile</t>
+  </si>
+  <si>
+    <t>OPQA-1196|OPQA-1200|OPQA-1199</t>
+  </si>
+  <si>
+    <t>Verify draft title,access and edit draft post from post modal, delete post from post modal</t>
   </si>
 </sst>
 </file>
@@ -1313,10 +1331,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75:E75"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2545,7 +2563,7 @@
       <c r="C72" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="D72" s="22" t="s">
+      <c r="D72" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E72" s="1"/>
@@ -2560,7 +2578,7 @@
       <c r="C73" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="D73" s="22" t="s">
+      <c r="D73" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E73" s="1"/>
@@ -2575,7 +2593,7 @@
       <c r="C74" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D74" s="22" t="s">
+      <c r="D74" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E74" s="1"/>
@@ -2590,10 +2608,40 @@
       <c r="C75" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="D75" s="22" t="s">
+      <c r="D75" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E75" s="1"/>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D76" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E76" s="1"/>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E77" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
made changes in Notifications test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Authoring.xlsx
+++ b/src/test/resources/xls/Authoring.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="275">
   <si>
     <t>TCID</t>
   </si>
@@ -840,6 +840,24 @@
   </si>
   <si>
     <t>Verify that timestamp is associated with the user generated posts.</t>
+  </si>
+  <si>
+    <t>Authoring75</t>
+  </si>
+  <si>
+    <t>Authoring76</t>
+  </si>
+  <si>
+    <t>OPQA-1195|OPQA-1313|OPQA-1312|OPQA-1090|OPQA-1201</t>
+  </si>
+  <si>
+    <t>Verify saving post as draft, accessing it for edit from profile,delete post from prfile</t>
+  </si>
+  <si>
+    <t>OPQA-1196|OPQA-1200|OPQA-1199</t>
+  </si>
+  <si>
+    <t>Verify draft title,access and edit draft post from post modal, delete post from post modal</t>
   </si>
 </sst>
 </file>
@@ -1313,10 +1331,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75:E75"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2545,7 +2563,7 @@
       <c r="C72" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="D72" s="22" t="s">
+      <c r="D72" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E72" s="1"/>
@@ -2560,7 +2578,7 @@
       <c r="C73" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="D73" s="22" t="s">
+      <c r="D73" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E73" s="1"/>
@@ -2575,7 +2593,7 @@
       <c r="C74" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D74" s="22" t="s">
+      <c r="D74" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E74" s="1"/>
@@ -2590,10 +2608,40 @@
       <c r="C75" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="D75" s="22" t="s">
+      <c r="D75" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E75" s="1"/>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D76" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E76" s="1"/>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E77" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Fixed search test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Authoring.xlsx
+++ b/src/test/resources/xls/Authoring.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="275">
   <si>
     <t>TCID</t>
   </si>
@@ -840,6 +840,24 @@
   </si>
   <si>
     <t>Verify that timestamp is associated with the user generated posts.</t>
+  </si>
+  <si>
+    <t>Authoring75</t>
+  </si>
+  <si>
+    <t>Authoring76</t>
+  </si>
+  <si>
+    <t>OPQA-1195|OPQA-1313|OPQA-1312|OPQA-1090|OPQA-1201</t>
+  </si>
+  <si>
+    <t>Verify saving post as draft, accessing it for edit from profile,delete post from prfile</t>
+  </si>
+  <si>
+    <t>OPQA-1196|OPQA-1200|OPQA-1199</t>
+  </si>
+  <si>
+    <t>Verify draft title,access and edit draft post from post modal, delete post from post modal</t>
   </si>
 </sst>
 </file>
@@ -1313,10 +1331,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75:E75"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2545,7 +2563,7 @@
       <c r="C72" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="D72" s="22" t="s">
+      <c r="D72" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E72" s="1"/>
@@ -2560,7 +2578,7 @@
       <c r="C73" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="D73" s="22" t="s">
+      <c r="D73" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E73" s="1"/>
@@ -2575,7 +2593,7 @@
       <c r="C74" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D74" s="22" t="s">
+      <c r="D74" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E74" s="1"/>
@@ -2590,10 +2608,40 @@
       <c r="C75" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="D75" s="22" t="s">
+      <c r="D75" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E75" s="1"/>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D76" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E76" s="1"/>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E77" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Increasing dynamic wait time
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Authoring.xlsx
+++ b/src/test/resources/xls/Authoring.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Test Case Steps" sheetId="4" r:id="rId2"/>
     <sheet name="Authoring1" sheetId="5" r:id="rId3"/>
-    <sheet name="Authoring8" sheetId="6" r:id="rId4"/>
-    <sheet name="Authoring9" sheetId="7" r:id="rId5"/>
-    <sheet name="Authoring10" sheetId="8" r:id="rId6"/>
-    <sheet name="Authoring23" sheetId="9" r:id="rId7"/>
-    <sheet name="Authoring46" sheetId="10" r:id="rId8"/>
+    <sheet name="Authoring46" sheetId="15" r:id="rId4"/>
+    <sheet name="Authoring8" sheetId="6" r:id="rId5"/>
+    <sheet name="Authoring9" sheetId="7" r:id="rId6"/>
+    <sheet name="Authoring10" sheetId="8" r:id="rId7"/>
+    <sheet name="Authoring23" sheetId="9" r:id="rId8"/>
     <sheet name="Authoring25" sheetId="11" r:id="rId9"/>
     <sheet name="Authoring30" sheetId="12" r:id="rId10"/>
     <sheet name="Authoring31" sheetId="13" r:id="rId11"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="274">
   <si>
     <t>TCID</t>
   </si>
@@ -144,9 +144,6 @@
     <t>&lt;li&gt;Coffee&lt;/li&gt;
 &lt;li&gt;Tea&lt;/li&gt;
 &lt;li&gt;Milk&lt;/li&gt;</t>
-  </si>
-  <si>
-    <t>Comments must have at least two characters, Please edit your comment.</t>
   </si>
   <si>
     <t xml:space="preserve">Verify that user Is able to comment on any article and validate the comment count increment </t>
@@ -1333,7 +1330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A48" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D75"/>
     </sheetView>
   </sheetViews>
@@ -1351,7 +1348,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>1</v>
@@ -1365,693 +1362,693 @@
     </row>
     <row r="2" spans="1:5" ht="25.5">
       <c r="A2" s="18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="25.5">
       <c r="A3" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="25.5">
       <c r="A4" s="18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="18" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B5" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>52</v>
-      </c>
       <c r="D5" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B6" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="18" t="s">
-        <v>54</v>
-      </c>
       <c r="D6" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="25.5">
       <c r="A7" s="18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B7" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>56</v>
-      </c>
       <c r="D7" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="25.5">
       <c r="A8" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="25.5">
       <c r="A9" s="18" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B9" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="18" t="s">
-        <v>59</v>
-      </c>
       <c r="D9" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B10" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="18" t="s">
-        <v>61</v>
-      </c>
       <c r="D10" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B11" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="18" t="s">
-        <v>63</v>
-      </c>
       <c r="D11" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D13" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D21" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B24" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="18" t="s">
-        <v>77</v>
-      </c>
       <c r="D24" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B25" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="C25" s="18" t="s">
-        <v>79</v>
-      </c>
       <c r="D25" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B26" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="C26" s="18" t="s">
-        <v>81</v>
-      </c>
       <c r="D26" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B27" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="C27" s="18" t="s">
-        <v>83</v>
-      </c>
       <c r="D27" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="25.5">
       <c r="A28" s="18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D28" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="25.5">
       <c r="A29" s="18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B29" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="C29" s="18" t="s">
-        <v>86</v>
-      </c>
       <c r="D29" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B30" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="C30" s="18" t="s">
-        <v>88</v>
-      </c>
       <c r="D30" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="25.5">
       <c r="A31" s="18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D31" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="25.5">
       <c r="A32" s="18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D32" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B33" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="C33" s="18" t="s">
-        <v>92</v>
-      </c>
       <c r="D33" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D34" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D35" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D36" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D37" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="25.5">
       <c r="A38" s="18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D38" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="25.5">
       <c r="A39" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D39" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B40" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="C40" s="18" t="s">
-        <v>98</v>
-      </c>
       <c r="D40" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B41" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C41" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C41" s="18" t="s">
-        <v>100</v>
-      </c>
       <c r="D41" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B42" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="D42" s="18" t="s">
         <v>3</v>
@@ -2062,268 +2059,268 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="18" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B43" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="D43" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B44" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="D44" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B45" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="D45" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B46" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D46" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B47" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="D47" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B48" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="D48" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B49" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="D49" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B50" s="20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D50" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B51" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D51" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B52" s="20" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D52" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="18" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B53" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D53" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B54" s="20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D54" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B55" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D55" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B56" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D56" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="18" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B57" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D57" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="18" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B58" s="20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D58" s="18" t="s">
         <v>3</v>
@@ -2334,217 +2331,217 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="18" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B59" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="C59" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="C59" s="8" t="s">
-        <v>159</v>
-      </c>
       <c r="D59" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="18" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B60" s="20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D60" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="18" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>163</v>
-      </c>
       <c r="D61" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B62" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="D62" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="18" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>167</v>
-      </c>
       <c r="D63" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="30">
       <c r="A64" s="18" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D64" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C65" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>171</v>
-      </c>
       <c r="D65" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="45">
       <c r="A66" s="18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C66" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="C66" s="4" t="s">
-        <v>174</v>
-      </c>
       <c r="D66" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="18" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D67" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="18" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>178</v>
-      </c>
       <c r="D68" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="30">
       <c r="A69" s="18" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D69" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="18" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B70" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>182</v>
-      </c>
       <c r="D70" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B71" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>184</v>
       </c>
       <c r="D71" s="18" t="s">
         <v>3</v>
@@ -2555,13 +2552,13 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D72" s="18" t="s">
         <v>3</v>
@@ -2570,13 +2567,13 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="18" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D73" s="18" t="s">
         <v>3</v>
@@ -2585,13 +2582,13 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="18" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D74" s="18" t="s">
         <v>3</v>
@@ -2600,13 +2597,13 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B75" s="8" t="s">
         <v>266</v>
       </c>
-      <c r="B75" s="8" t="s">
+      <c r="C75" s="1" t="s">
         <v>267</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>268</v>
       </c>
       <c r="D75" s="18" t="s">
         <v>3</v>
@@ -2615,13 +2612,13 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B76" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="C76" s="1" t="s">
         <v>271</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>272</v>
       </c>
       <c r="D76" s="22" t="s">
         <v>3</v>
@@ -2630,13 +2627,13 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B77" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C77" s="1" t="s">
         <v>273</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>274</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>3</v>
@@ -2717,7 +2714,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>16</v>
@@ -2734,7 +2731,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2774,10 +2771,10 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>43</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>16</v>
@@ -2794,10 +2791,10 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
         <v>44</v>
-      </c>
-      <c r="B2" t="s">
-        <v>45</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2852,7 +2849,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -2866,7 +2863,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
@@ -2880,7 +2877,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
@@ -2894,7 +2891,7 @@
         <v>29</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>3</v>
@@ -2908,7 +2905,7 @@
         <v>30</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>3</v>
@@ -2922,7 +2919,7 @@
         <v>31</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>3</v>
@@ -3026,7 +3023,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>14</v>
@@ -3049,7 +3046,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3089,7 +3086,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>21</v>
@@ -3108,6 +3105,69 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="70.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="47.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -3227,7 +3287,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -3304,7 +3364,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -3415,72 +3475,6 @@
       </c>
       <c r="D7" s="1" t="s">
         <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F38"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="68.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="38" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75">
-      <c r="A2" s="10">
-        <v>1</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="10">
-        <v>1600</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" spans="5:5">
-      <c r="E38" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
code changes are done in TestUtil.java
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Authoring.xlsx
+++ b/src/test/resources/xls/Authoring.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900" firstSheet="5" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="275">
   <si>
     <t>TCID</t>
   </si>
@@ -855,12 +855,16 @@
   </si>
   <si>
     <t>Verify draft title,access and edit draft post from post modal, delete post from post modal</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -989,7 +993,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1028,9 +1032,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1330,17 +1331,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D75"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="70.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="39.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="70.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="6.8046875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="16" customFormat="1">
@@ -1388,7 +1389,7 @@
         <v>48</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E3" s="18" t="s">
         <v>113</v>
@@ -1405,7 +1406,7 @@
         <v>49</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E4" s="18" t="s">
         <v>113</v>
@@ -1422,7 +1423,7 @@
         <v>51</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E5" s="18" t="s">
         <v>113</v>
@@ -1439,7 +1440,7 @@
         <v>53</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>113</v>
@@ -1456,7 +1457,7 @@
         <v>55</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>113</v>
@@ -1473,7 +1474,7 @@
         <v>56</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E8" s="18" t="s">
         <v>113</v>
@@ -1490,7 +1491,7 @@
         <v>58</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E9" s="18" t="s">
         <v>113</v>
@@ -1507,7 +1508,7 @@
         <v>60</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E10" s="18" t="s">
         <v>113</v>
@@ -1524,7 +1525,7 @@
         <v>62</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E11" s="18" t="s">
         <v>113</v>
@@ -1541,7 +1542,7 @@
         <v>64</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E12" s="18" t="s">
         <v>113</v>
@@ -1558,7 +1559,7 @@
         <v>65</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E13" s="18" t="s">
         <v>113</v>
@@ -1575,7 +1576,7 @@
         <v>66</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E14" s="18" t="s">
         <v>113</v>
@@ -1592,7 +1593,7 @@
         <v>67</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E15" s="18" t="s">
         <v>113</v>
@@ -1609,7 +1610,7 @@
         <v>68</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E16" s="18" t="s">
         <v>113</v>
@@ -1626,7 +1627,7 @@
         <v>69</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E17" s="18" t="s">
         <v>113</v>
@@ -1643,7 +1644,7 @@
         <v>70</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E18" s="18" t="s">
         <v>113</v>
@@ -1660,7 +1661,7 @@
         <v>71</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E19" s="18" t="s">
         <v>113</v>
@@ -1677,7 +1678,7 @@
         <v>72</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E20" s="18" t="s">
         <v>113</v>
@@ -1694,7 +1695,7 @@
         <v>73</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>113</v>
@@ -1711,7 +1712,7 @@
         <v>123</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E22" s="18" t="s">
         <v>113</v>
@@ -1728,7 +1729,7 @@
         <v>74</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E23" s="18" t="s">
         <v>113</v>
@@ -1745,7 +1746,7 @@
         <v>76</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E24" s="18" t="s">
         <v>113</v>
@@ -1762,7 +1763,7 @@
         <v>78</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E25" s="18" t="s">
         <v>113</v>
@@ -1779,7 +1780,7 @@
         <v>80</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E26" s="18" t="s">
         <v>113</v>
@@ -1796,7 +1797,7 @@
         <v>82</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E27" s="18" t="s">
         <v>113</v>
@@ -1813,7 +1814,7 @@
         <v>83</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E28" s="18" t="s">
         <v>113</v>
@@ -1830,7 +1831,7 @@
         <v>85</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E29" s="18" t="s">
         <v>113</v>
@@ -1847,7 +1848,7 @@
         <v>87</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E30" s="18" t="s">
         <v>113</v>
@@ -1864,7 +1865,7 @@
         <v>128</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E31" s="18" t="s">
         <v>113</v>
@@ -1881,7 +1882,7 @@
         <v>129</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E32" s="18" t="s">
         <v>113</v>
@@ -1898,7 +1899,7 @@
         <v>91</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E33" s="18" t="s">
         <v>113</v>
@@ -1915,7 +1916,7 @@
         <v>92</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E34" s="18" t="s">
         <v>113</v>
@@ -1932,7 +1933,7 @@
         <v>93</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E35" s="18" t="s">
         <v>113</v>
@@ -1949,7 +1950,7 @@
         <v>94</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E36" s="18" t="s">
         <v>113</v>
@@ -1966,7 +1967,7 @@
         <v>95</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E37" s="18" t="s">
         <v>113</v>
@@ -1983,7 +1984,7 @@
         <v>126</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E38" s="18" t="s">
         <v>113</v>
@@ -2000,7 +2001,7 @@
         <v>127</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E39" s="18" t="s">
         <v>113</v>
@@ -2017,7 +2018,7 @@
         <v>97</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E40" s="18" t="s">
         <v>113</v>
@@ -2034,7 +2035,7 @@
         <v>99</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E41" s="18" t="s">
         <v>113</v>
@@ -2051,7 +2052,7 @@
         <v>102</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>28</v>
@@ -2068,7 +2069,7 @@
         <v>104</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>113</v>
@@ -2085,7 +2086,7 @@
         <v>106</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>113</v>
@@ -2102,7 +2103,7 @@
         <v>108</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>113</v>
@@ -2119,7 +2120,7 @@
         <v>109</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>113</v>
@@ -2136,7 +2137,7 @@
         <v>112</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>113</v>
@@ -2153,7 +2154,7 @@
         <v>137</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>113</v>
@@ -2170,7 +2171,7 @@
         <v>139</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>113</v>
@@ -2187,7 +2188,7 @@
         <v>140</v>
       </c>
       <c r="D50" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>113</v>
@@ -2204,7 +2205,7 @@
         <v>142</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>113</v>
@@ -2221,7 +2222,7 @@
         <v>144</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>113</v>
@@ -2238,7 +2239,7 @@
         <v>151</v>
       </c>
       <c r="D53" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>113</v>
@@ -2255,7 +2256,7 @@
         <v>152</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>113</v>
@@ -2272,7 +2273,7 @@
         <v>153</v>
       </c>
       <c r="D55" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>113</v>
@@ -2289,7 +2290,7 @@
         <v>154</v>
       </c>
       <c r="D56" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>113</v>
@@ -2306,7 +2307,7 @@
         <v>155</v>
       </c>
       <c r="D57" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>113</v>
@@ -2323,7 +2324,7 @@
         <v>156</v>
       </c>
       <c r="D58" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>28</v>
@@ -2340,7 +2341,7 @@
         <v>158</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>113</v>
@@ -2357,7 +2358,7 @@
         <v>159</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>113</v>
@@ -2374,7 +2375,7 @@
         <v>162</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>113</v>
@@ -2391,7 +2392,7 @@
         <v>164</v>
       </c>
       <c r="D62" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>113</v>
@@ -2408,7 +2409,7 @@
         <v>166</v>
       </c>
       <c r="D63" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>113</v>
@@ -2425,7 +2426,7 @@
         <v>167</v>
       </c>
       <c r="D64" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E64" s="8" t="s">
         <v>113</v>
@@ -2442,7 +2443,7 @@
         <v>170</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>113</v>
@@ -2459,7 +2460,7 @@
         <v>173</v>
       </c>
       <c r="D66" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>113</v>
@@ -2476,7 +2477,7 @@
         <v>174</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>113</v>
@@ -2493,7 +2494,7 @@
         <v>177</v>
       </c>
       <c r="D68" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>113</v>
@@ -2510,7 +2511,7 @@
         <v>178</v>
       </c>
       <c r="D69" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>113</v>
@@ -2527,7 +2528,7 @@
         <v>181</v>
       </c>
       <c r="D70" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>113</v>
@@ -2544,7 +2545,7 @@
         <v>183</v>
       </c>
       <c r="D71" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>28</v>
@@ -2561,7 +2562,7 @@
         <v>262</v>
       </c>
       <c r="D72" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E72" s="1"/>
     </row>
@@ -2576,7 +2577,7 @@
         <v>263</v>
       </c>
       <c r="D73" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E73" s="1"/>
     </row>
@@ -2591,7 +2592,7 @@
         <v>264</v>
       </c>
       <c r="D74" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E74" s="1"/>
     </row>
@@ -2606,7 +2607,7 @@
         <v>267</v>
       </c>
       <c r="D75" s="18" t="s">
-        <v>3</v>
+        <v>274</v>
       </c>
       <c r="E75" s="1"/>
     </row>
@@ -2620,8 +2621,8 @@
       <c r="C76" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="D76" s="22" t="s">
-        <v>3</v>
+      <c r="D76" s="18" t="s">
+        <v>274</v>
       </c>
       <c r="E76" s="1"/>
     </row>
@@ -2635,8 +2636,8 @@
       <c r="C77" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="D77" s="1" t="s">
-        <v>3</v>
+      <c r="D77" s="18" t="s">
+        <v>274</v>
       </c>
       <c r="E77" s="1"/>
     </row>
@@ -2708,8 +2709,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="56" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="56.0" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2762,11 +2763,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="55" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="43.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="55.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="43.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2819,16 +2820,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="31.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="26.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2944,10 +2945,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="45.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="83.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="45.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="83.5703125" collapsed="true"/>
+    <col min="4" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2985,12 +2986,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3052,11 +3053,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="70.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="47.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="70.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="47.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3115,11 +3116,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="70.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="47.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="70.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="47.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3178,10 +3179,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="54.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="11" customFormat="1">
@@ -3298,10 +3299,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="61.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="51.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="61.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3375,9 +3376,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="59.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="59.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3493,10 +3494,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="35.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="35.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>

<commit_message>
taking latest changes and appending changes in TestUtil.java
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Authoring.xlsx
+++ b/src/test/resources/xls/Authoring.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900" firstSheet="5" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -989,7 +989,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1028,9 +1028,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1330,8 +1327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D75"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2620,7 +2617,7 @@
       <c r="C76" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="D76" s="22" t="s">
+      <c r="D76" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E76" s="1"/>
@@ -2635,7 +2632,7 @@
       <c r="C77" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="D77" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E77" s="1"/>
@@ -2819,7 +2816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added 2 new watchlist test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Authoring.xlsx
+++ b/src/test/resources/xls/Authoring.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -552,10 +552,6 @@
     <t>OPQA-1190</t>
   </si>
   <si>
-    <t>Verify that Publish a Post option is displayed in Home page and all Record view 
-pages like Article,Post ,Patent</t>
-  </si>
-  <si>
     <t>Verfiy that the Drafts Post tab is not displayed when there are no draft posts</t>
   </si>
   <si>
@@ -858,6 +854,9 @@
   </si>
   <si>
     <t>Comments must have at least two characters, Please edit your comment.</t>
+  </si>
+  <si>
+    <t>Verify that Publish a Post option is displayed in the header section</t>
   </si>
 </sst>
 </file>
@@ -1330,8 +1329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D77"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1362,10 +1361,10 @@
     </row>
     <row r="2" spans="1:5" ht="25.5">
       <c r="A2" s="18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>38</v>
@@ -1379,10 +1378,10 @@
     </row>
     <row r="3" spans="1:5" ht="25.5">
       <c r="A3" s="18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>48</v>
@@ -1396,10 +1395,10 @@
     </row>
     <row r="4" spans="1:5" ht="25.5">
       <c r="A4" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>49</v>
@@ -1413,7 +1412,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B5" s="19" t="s">
         <v>50</v>
@@ -1430,7 +1429,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="18" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B6" s="19" t="s">
         <v>52</v>
@@ -1447,7 +1446,7 @@
     </row>
     <row r="7" spans="1:5" ht="25.5">
       <c r="A7" s="18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B7" s="19" t="s">
         <v>54</v>
@@ -1464,7 +1463,7 @@
     </row>
     <row r="8" spans="1:5" ht="25.5">
       <c r="A8" s="18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B8" s="20" t="s">
         <v>114</v>
@@ -1481,7 +1480,7 @@
     </row>
     <row r="9" spans="1:5" ht="25.5">
       <c r="A9" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>57</v>
@@ -1498,7 +1497,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="18" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B10" s="19" t="s">
         <v>59</v>
@@ -1515,7 +1514,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B11" s="19" t="s">
         <v>61</v>
@@ -1532,7 +1531,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B12" s="20" t="s">
         <v>116</v>
@@ -1549,7 +1548,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B13" s="20" t="s">
         <v>115</v>
@@ -1566,7 +1565,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B14" s="19" t="s">
         <v>63</v>
@@ -1583,7 +1582,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B15" s="20" t="s">
         <v>117</v>
@@ -1600,7 +1599,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B16" s="20" t="s">
         <v>118</v>
@@ -1617,10 +1616,10 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>69</v>
@@ -1634,7 +1633,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B18" s="20" t="s">
         <v>119</v>
@@ -1651,7 +1650,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B19" s="20" t="s">
         <v>120</v>
@@ -1668,7 +1667,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B20" s="20" t="s">
         <v>121</v>
@@ -1685,7 +1684,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B21" s="20" t="s">
         <v>122</v>
@@ -1702,7 +1701,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B22" s="20" t="s">
         <v>124</v>
@@ -1719,10 +1718,10 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C23" s="18" t="s">
         <v>74</v>
@@ -1736,7 +1735,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B24" s="19" t="s">
         <v>75</v>
@@ -1753,7 +1752,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B25" s="19" t="s">
         <v>77</v>
@@ -1770,7 +1769,7 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B26" s="19" t="s">
         <v>79</v>
@@ -1787,7 +1786,7 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B27" s="19" t="s">
         <v>81</v>
@@ -1804,7 +1803,7 @@
     </row>
     <row r="28" spans="1:5" ht="25.5">
       <c r="A28" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B28" s="20" t="s">
         <v>125</v>
@@ -1821,7 +1820,7 @@
     </row>
     <row r="29" spans="1:5" ht="25.5">
       <c r="A29" s="18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B29" s="19" t="s">
         <v>84</v>
@@ -1838,7 +1837,7 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B30" s="19" t="s">
         <v>86</v>
@@ -1855,7 +1854,7 @@
     </row>
     <row r="31" spans="1:5" ht="25.5">
       <c r="A31" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B31" s="19" t="s">
         <v>88</v>
@@ -1872,7 +1871,7 @@
     </row>
     <row r="32" spans="1:5" ht="25.5">
       <c r="A32" s="18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B32" s="19" t="s">
         <v>89</v>
@@ -1889,7 +1888,7 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B33" s="19" t="s">
         <v>90</v>
@@ -1906,7 +1905,7 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B34" s="20" t="s">
         <v>130</v>
@@ -1923,7 +1922,7 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B35" s="20" t="s">
         <v>133</v>
@@ -1940,7 +1939,7 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B36" s="20" t="s">
         <v>134</v>
@@ -1957,7 +1956,7 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B37" s="20" t="s">
         <v>131</v>
@@ -1974,7 +1973,7 @@
     </row>
     <row r="38" spans="1:5" ht="25.5">
       <c r="A38" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B38" s="20" t="s">
         <v>132</v>
@@ -1991,7 +1990,7 @@
     </row>
     <row r="39" spans="1:5" ht="25.5">
       <c r="A39" s="18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B39" s="20" t="s">
         <v>135</v>
@@ -2008,7 +2007,7 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B40" s="19" t="s">
         <v>96</v>
@@ -2025,7 +2024,7 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B41" s="19" t="s">
         <v>98</v>
@@ -2042,7 +2041,7 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B42" s="19" t="s">
         <v>101</v>
@@ -2059,7 +2058,7 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B43" s="19" t="s">
         <v>103</v>
@@ -2076,7 +2075,7 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="18" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B44" s="19" t="s">
         <v>105</v>
@@ -2093,7 +2092,7 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B45" s="20" t="s">
         <v>107</v>
@@ -2110,7 +2109,7 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B46" s="20" t="s">
         <v>110</v>
@@ -2127,7 +2126,7 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B47" s="20" t="s">
         <v>111</v>
@@ -2144,7 +2143,7 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B48" s="20" t="s">
         <v>136</v>
@@ -2161,7 +2160,7 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B49" s="20" t="s">
         <v>138</v>
@@ -2178,7 +2177,7 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B50" s="20" t="s">
         <v>141</v>
@@ -2195,7 +2194,7 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B51" s="20" t="s">
         <v>143</v>
@@ -2212,7 +2211,7 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B52" s="20" t="s">
         <v>171</v>
@@ -2229,7 +2228,7 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B53" s="20" t="s">
         <v>149</v>
@@ -2246,7 +2245,7 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="18" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B54" s="20" t="s">
         <v>148</v>
@@ -2263,7 +2262,7 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B55" s="20" t="s">
         <v>150</v>
@@ -2280,7 +2279,7 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B56" s="20" t="s">
         <v>145</v>
@@ -2297,7 +2296,7 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B57" s="20" t="s">
         <v>146</v>
@@ -2314,7 +2313,7 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="18" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B58" s="20" t="s">
         <v>147</v>
@@ -2331,7 +2330,7 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="18" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B59" s="20" t="s">
         <v>157</v>
@@ -2348,7 +2347,7 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="18" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B60" s="20" t="s">
         <v>160</v>
@@ -2365,7 +2364,7 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="18" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>161</v>
@@ -2382,7 +2381,7 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="18" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>163</v>
@@ -2399,7 +2398,7 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>165</v>
@@ -2416,7 +2415,7 @@
     </row>
     <row r="64" spans="1:5" ht="30">
       <c r="A64" s="18" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B64" s="8" t="s">
         <v>168</v>
@@ -2433,7 +2432,7 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="18" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>169</v>
@@ -2448,15 +2447,15 @@
         <v>113</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="45">
+    <row r="66" spans="1:5">
       <c r="A66" s="18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>172</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>173</v>
+        <v>274</v>
       </c>
       <c r="D66" s="18" t="s">
         <v>3</v>
@@ -2467,13 +2466,13 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D67" s="18" t="s">
         <v>3</v>
@@ -2484,13 +2483,13 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="18" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>177</v>
       </c>
       <c r="D68" s="18" t="s">
         <v>3</v>
@@ -2501,13 +2500,13 @@
     </row>
     <row r="69" spans="1:5" ht="30">
       <c r="A69" s="18" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D69" s="18" t="s">
         <v>3</v>
@@ -2518,13 +2517,13 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="18" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B70" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>181</v>
       </c>
       <c r="D70" s="18" t="s">
         <v>3</v>
@@ -2535,13 +2534,13 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="18" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B71" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="D71" s="18" t="s">
         <v>3</v>
@@ -2552,13 +2551,13 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B72" s="8" t="s">
         <v>157</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D72" s="18" t="s">
         <v>3</v>
@@ -2567,13 +2566,13 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D73" s="18" t="s">
         <v>3</v>
@@ -2582,13 +2581,13 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="18" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B74" s="8" t="s">
         <v>110</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D74" s="18" t="s">
         <v>3</v>
@@ -2597,13 +2596,13 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B75" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="B75" s="8" t="s">
+      <c r="C75" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>267</v>
       </c>
       <c r="D75" s="18" t="s">
         <v>3</v>
@@ -2612,13 +2611,13 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B76" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="C76" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>271</v>
       </c>
       <c r="D76" s="18" t="s">
         <v>3</v>
@@ -2627,13 +2626,13 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B77" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C77" s="1" t="s">
         <v>272</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>273</v>
       </c>
       <c r="D77" s="18" t="s">
         <v>3</v>
@@ -3046,7 +3045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -3084,7 +3083,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Added new Watchlist test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Authoring.xlsx
+++ b/src/test/resources/xls/Authoring.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900" firstSheet="5" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Authoring30" sheetId="12" r:id="rId10"/>
     <sheet name="Authoring31" sheetId="13" r:id="rId11"/>
     <sheet name="PostProfanityWordCheckTest" sheetId="16" r:id="rId12"/>
+    <sheet name="deek_linking" sheetId="17" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Test Cases'!$A$1:$E$71</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="301">
   <si>
     <t>TCID</t>
   </si>
@@ -857,6 +858,84 @@
   </si>
   <si>
     <t>Verify that Publish a Post option is displayed in the header section</t>
+  </si>
+  <si>
+    <t>Authoring77</t>
+  </si>
+  <si>
+    <t>OPQA-2799|OPQA-2806|OPQA-2807</t>
+  </si>
+  <si>
+    <t>Verify that deep linking works fine for ARTICLES,POSTS,PATENTS with Neon login</t>
+  </si>
+  <si>
+    <t>Authoring78</t>
+  </si>
+  <si>
+    <t>OPQA-2832|OPQA-2832</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that deep linking works fine for ARTICLES,POSTS,PATENTS with Social login </t>
+  </si>
+  <si>
+    <t>Authoring79</t>
+  </si>
+  <si>
+    <t>OPQA-2830</t>
+  </si>
+  <si>
+    <t>Verify that deep linking works fine for ARTICLES,POSTS,PATENTS with Social login</t>
+  </si>
+  <si>
+    <t>Authoring80</t>
+  </si>
+  <si>
+    <t>OPQA-2929</t>
+  </si>
+  <si>
+    <t>Verify that user is able to share the post created by others via Google+</t>
+  </si>
+  <si>
+    <t>Authoring81</t>
+  </si>
+  <si>
+    <t>OPQA-2928</t>
+  </si>
+  <si>
+    <t>Verify that user is able to share their posts on Google+</t>
+  </si>
+  <si>
+    <t>Authoring82</t>
+  </si>
+  <si>
+    <t>OPQA-2931</t>
+  </si>
+  <si>
+    <t>Verify that user is able to share articles on Google+</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>recordType</t>
+  </si>
+  <si>
+    <t>/#/wos/491710049WOS1</t>
+  </si>
+  <si>
+    <t>ARTICLE</t>
+  </si>
+  <si>
+    <t>/#/posts/8b28ac5a-db05-4a0d-8da9-3553ebbcd3f2</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>/#/patents/US20070269858A120071122</t>
+  </si>
+  <si>
+    <t>PATENT</t>
   </si>
 </sst>
 </file>
@@ -991,7 +1070,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1031,6 +1110,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1327,10 +1409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView topLeftCell="A62" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78:E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2638,6 +2720,96 @@
         <v>3</v>
       </c>
       <c r="E77" s="1"/>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="D78" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E78" s="1"/>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="C79" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="D79" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E79" s="1"/>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="C80" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="D80" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E80" s="1"/>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B81" s="20" t="s">
+        <v>285</v>
+      </c>
+      <c r="C81" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="D81" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E81" s="1"/>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B82" s="20" t="s">
+        <v>288</v>
+      </c>
+      <c r="C82" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="D82" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E82" s="1"/>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B83" s="20" t="s">
+        <v>291</v>
+      </c>
+      <c r="C83" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="D83" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E83" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2691,9 +2863,12 @@
     <hyperlink ref="B59" r:id="rId48" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1074"/>
     <hyperlink ref="B60" r:id="rId49" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1076"/>
     <hyperlink ref="B2" r:id="rId50" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-236"/>
+    <hyperlink ref="B83" r:id="rId51" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-2931"/>
+    <hyperlink ref="B81" r:id="rId52" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-2929"/>
+    <hyperlink ref="B82" r:id="rId53" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-2928"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId51"/>
+  <pageSetup orientation="portrait" r:id="rId54"/>
 </worksheet>
 </file>
 
@@ -2933,6 +3108,82 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="65.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="22" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>297</v>
+      </c>
+      <c r="B3" t="s">
+        <v>298</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>299</v>
+      </c>
+      <c r="B4" t="s">
+        <v>300</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>

</xml_diff>

<commit_message>
Scripted new authoring scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Authoring.xlsx
+++ b/src/test/resources/xls/Authoring.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="313">
   <si>
     <t>TCID</t>
   </si>
@@ -1450,8 +1450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2683,7 +2683,9 @@
       <c r="D72" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E72" s="1"/>
+      <c r="E72" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="18" t="s">

</xml_diff>

<commit_message>
Enabled all the tests.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Authoring.xlsx
+++ b/src/test/resources/xls/Authoring.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="319">
   <si>
     <t>TCID</t>
   </si>
@@ -991,9 +991,6 @@
   <si>
     <t>1.Verify that spam check and unsupported tag validations are not done on draft post
 2.Verify that spam check and unsupported tag validations are done when user publishes the draft post</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -1470,7 +1467,7 @@
   <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A59" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+      <selection activeCell="D2" sqref="D2:D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1510,7 +1507,7 @@
         <v>38</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>112</v>
@@ -1527,7 +1524,7 @@
         <v>48</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E3" s="18" t="s">
         <v>112</v>
@@ -1544,7 +1541,7 @@
         <v>49</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E4" s="18" t="s">
         <v>112</v>
@@ -1561,7 +1558,7 @@
         <v>51</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E5" s="18" t="s">
         <v>112</v>
@@ -1578,7 +1575,7 @@
         <v>53</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>112</v>
@@ -1595,7 +1592,7 @@
         <v>55</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>112</v>
@@ -1612,7 +1609,7 @@
         <v>56</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E8" s="18" t="s">
         <v>112</v>
@@ -1629,7 +1626,7 @@
         <v>58</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E9" s="18" t="s">
         <v>112</v>
@@ -1646,7 +1643,7 @@
         <v>60</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E10" s="18" t="s">
         <v>112</v>
@@ -1663,7 +1660,7 @@
         <v>62</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E11" s="18" t="s">
         <v>112</v>
@@ -1680,7 +1677,7 @@
         <v>64</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E12" s="18" t="s">
         <v>112</v>
@@ -1697,7 +1694,7 @@
         <v>65</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E13" s="18" t="s">
         <v>112</v>
@@ -1714,7 +1711,7 @@
         <v>66</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E14" s="18" t="s">
         <v>112</v>
@@ -1731,7 +1728,7 @@
         <v>67</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E15" s="18" t="s">
         <v>112</v>
@@ -1748,7 +1745,7 @@
         <v>68</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E16" s="18" t="s">
         <v>112</v>
@@ -1765,7 +1762,7 @@
         <v>69</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E17" s="18" t="s">
         <v>112</v>
@@ -1782,7 +1779,7 @@
         <v>70</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E18" s="18" t="s">
         <v>112</v>
@@ -1799,7 +1796,7 @@
         <v>71</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E19" s="18" t="s">
         <v>112</v>
@@ -1816,7 +1813,7 @@
         <v>72</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E20" s="18" t="s">
         <v>112</v>
@@ -1833,7 +1830,7 @@
         <v>73</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>112</v>
@@ -1850,7 +1847,7 @@
         <v>122</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E22" s="18" t="s">
         <v>112</v>
@@ -1867,7 +1864,7 @@
         <v>74</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E23" s="18" t="s">
         <v>112</v>
@@ -1884,7 +1881,7 @@
         <v>76</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E24" s="18" t="s">
         <v>112</v>
@@ -1901,7 +1898,7 @@
         <v>78</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E25" s="18" t="s">
         <v>112</v>
@@ -1918,7 +1915,7 @@
         <v>80</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E26" s="18" t="s">
         <v>112</v>
@@ -1935,7 +1932,7 @@
         <v>82</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E27" s="18" t="s">
         <v>112</v>
@@ -1952,7 +1949,7 @@
         <v>83</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E28" s="18" t="s">
         <v>112</v>
@@ -1969,7 +1966,7 @@
         <v>85</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E29" s="18" t="s">
         <v>112</v>
@@ -1986,7 +1983,7 @@
         <v>86</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E30" s="18" t="s">
         <v>112</v>
@@ -2003,7 +2000,7 @@
         <v>127</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E31" s="18" t="s">
         <v>112</v>
@@ -2020,7 +2017,7 @@
         <v>128</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E32" s="18" t="s">
         <v>112</v>
@@ -2037,7 +2034,7 @@
         <v>90</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E33" s="18" t="s">
         <v>112</v>
@@ -2054,7 +2051,7 @@
         <v>91</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E34" s="18" t="s">
         <v>112</v>
@@ -2071,7 +2068,7 @@
         <v>92</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E35" s="18" t="s">
         <v>112</v>
@@ -2088,7 +2085,7 @@
         <v>93</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E36" s="18" t="s">
         <v>112</v>
@@ -2105,7 +2102,7 @@
         <v>94</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E37" s="18" t="s">
         <v>112</v>
@@ -2122,7 +2119,7 @@
         <v>125</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E38" s="18" t="s">
         <v>28</v>
@@ -2139,7 +2136,7 @@
         <v>126</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E39" s="18" t="s">
         <v>112</v>
@@ -2156,7 +2153,7 @@
         <v>96</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E40" s="18" t="s">
         <v>112</v>
@@ -2173,7 +2170,7 @@
         <v>98</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E41" s="18" t="s">
         <v>112</v>
@@ -2190,7 +2187,7 @@
         <v>101</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>28</v>
@@ -2207,7 +2204,7 @@
         <v>103</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>112</v>
@@ -2224,7 +2221,7 @@
         <v>105</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>112</v>
@@ -2241,7 +2238,7 @@
         <v>107</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>112</v>
@@ -2258,7 +2255,7 @@
         <v>108</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>112</v>
@@ -2275,7 +2272,7 @@
         <v>111</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>112</v>
@@ -2292,7 +2289,7 @@
         <v>136</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>112</v>
@@ -2309,7 +2306,7 @@
         <v>138</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>112</v>
@@ -2326,7 +2323,7 @@
         <v>139</v>
       </c>
       <c r="D50" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>112</v>
@@ -2343,7 +2340,7 @@
         <v>141</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>112</v>
@@ -2360,7 +2357,7 @@
         <v>142</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>112</v>
@@ -2377,7 +2374,7 @@
         <v>149</v>
       </c>
       <c r="D53" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>112</v>
@@ -2394,7 +2391,7 @@
         <v>150</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>112</v>
@@ -2411,7 +2408,7 @@
         <v>151</v>
       </c>
       <c r="D55" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>112</v>
@@ -2428,7 +2425,7 @@
         <v>152</v>
       </c>
       <c r="D56" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>112</v>
@@ -2445,7 +2442,7 @@
         <v>153</v>
       </c>
       <c r="D57" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>112</v>
@@ -2462,7 +2459,7 @@
         <v>154</v>
       </c>
       <c r="D58" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>28</v>
@@ -2479,7 +2476,7 @@
         <v>156</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>112</v>
@@ -2496,7 +2493,7 @@
         <v>157</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>112</v>
@@ -2513,7 +2510,7 @@
         <v>160</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>112</v>
@@ -2530,7 +2527,7 @@
         <v>162</v>
       </c>
       <c r="D62" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>112</v>
@@ -2547,7 +2544,7 @@
         <v>164</v>
       </c>
       <c r="D63" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>112</v>
@@ -2564,7 +2561,7 @@
         <v>165</v>
       </c>
       <c r="D64" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E64" s="8" t="s">
         <v>112</v>
@@ -2581,7 +2578,7 @@
         <v>168</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>112</v>
@@ -2598,7 +2595,7 @@
         <v>272</v>
       </c>
       <c r="D66" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>112</v>
@@ -2615,7 +2612,7 @@
         <v>171</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>112</v>
@@ -2632,7 +2629,7 @@
         <v>174</v>
       </c>
       <c r="D68" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>112</v>
@@ -2649,7 +2646,7 @@
         <v>175</v>
       </c>
       <c r="D69" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>112</v>
@@ -2666,7 +2663,7 @@
         <v>178</v>
       </c>
       <c r="D70" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>112</v>
@@ -2683,7 +2680,7 @@
         <v>180</v>
       </c>
       <c r="D71" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>28</v>
@@ -2700,7 +2697,7 @@
         <v>259</v>
       </c>
       <c r="D72" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>112</v>
@@ -2717,7 +2714,7 @@
         <v>260</v>
       </c>
       <c r="D73" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E73" s="1"/>
     </row>
@@ -2732,7 +2729,7 @@
         <v>261</v>
       </c>
       <c r="D74" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E74" s="1"/>
     </row>
@@ -2747,7 +2744,7 @@
         <v>264</v>
       </c>
       <c r="D75" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E75" s="1"/>
     </row>
@@ -2762,7 +2759,7 @@
         <v>268</v>
       </c>
       <c r="D76" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E76" s="1"/>
     </row>
@@ -2777,7 +2774,7 @@
         <v>270</v>
       </c>
       <c r="D77" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E77" s="1"/>
     </row>
@@ -2792,7 +2789,7 @@
         <v>275</v>
       </c>
       <c r="D78" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E78" s="1"/>
     </row>
@@ -2807,7 +2804,7 @@
         <v>278</v>
       </c>
       <c r="D79" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E79" s="1"/>
     </row>
@@ -2822,7 +2819,7 @@
         <v>281</v>
       </c>
       <c r="D80" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E80" s="1"/>
     </row>
@@ -2852,7 +2849,7 @@
         <v>287</v>
       </c>
       <c r="D82" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E82" s="1"/>
     </row>
@@ -2867,7 +2864,7 @@
         <v>290</v>
       </c>
       <c r="D83" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E83" s="1"/>
     </row>
@@ -2882,7 +2879,7 @@
         <v>301</v>
       </c>
       <c r="D84" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E84" s="1"/>
     </row>
@@ -2897,7 +2894,7 @@
         <v>307</v>
       </c>
       <c r="D85" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E85" s="1"/>
     </row>
@@ -2912,7 +2909,7 @@
         <v>304</v>
       </c>
       <c r="D86" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E86" s="1"/>
     </row>
@@ -2927,7 +2924,7 @@
         <v>310</v>
       </c>
       <c r="D87" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E87" s="1"/>
     </row>
@@ -2942,7 +2939,7 @@
         <v>315</v>
       </c>
       <c r="D88" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E88" s="1"/>
     </row>
@@ -2957,7 +2954,7 @@
         <v>318</v>
       </c>
       <c r="D89" s="18" t="s">
-        <v>319</v>
+        <v>3</v>
       </c>
       <c r="E89" s="1"/>
     </row>

</xml_diff>

<commit_message>
modified authoring xls file
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Authoring.xlsx
+++ b/src/test/resources/xls/Authoring.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="319">
   <si>
     <t>TCID</t>
   </si>
@@ -1434,7 +1434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A58" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -3659,10 +3659,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3689,7 +3689,7 @@
     </row>
     <row r="2" spans="1:4" ht="15.75">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>36</v>
@@ -3701,9 +3701,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75">
-      <c r="A3" s="1" t="s">
-        <v>34</v>
+    <row r="3" spans="1:4" ht="45">
+      <c r="A3" s="15" t="s">
+        <v>37</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>36</v>
@@ -3712,20 +3712,6 @@
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="45">
-      <c r="A4" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added changes to Authoring 81,82,83
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Authoring.xlsx
+++ b/src/test/resources/xls/Authoring.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="320">
   <si>
     <t>TCID</t>
   </si>
@@ -991,12 +991,16 @@
   </si>
   <si>
     <t>&lt;div&gt;Adding comment with div tag&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -1440,11 +1444,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="87.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="39.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="87.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="6.8046875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="16" customFormat="1">
@@ -2090,7 +2094,7 @@
         <v>3</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>28</v>
+        <v>319</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="25.5">
@@ -3001,8 +3005,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="56" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="56.0" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3055,11 +3059,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="55" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="43.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="55.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="43.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3118,10 +3122,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="26.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3237,9 +3241,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="65.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="65.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3313,10 +3317,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="45.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="83.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="45.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="83.5703125" collapsed="true"/>
+    <col min="4" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3354,12 +3358,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3421,11 +3425,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="70.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="47.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="70.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="47.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3484,11 +3488,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="70.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="47.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="70.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="47.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3547,10 +3551,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="54.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="11" customFormat="1">
@@ -3667,10 +3671,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="61.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="51.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="61.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3744,9 +3748,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="59.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="59.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3862,10 +3866,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="35.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="35.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>

<commit_message>
Authoring test script fixes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Authoring.xlsx
+++ b/src/test/resources/xls/Authoring.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="18330" windowHeight="4290" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -25,11 +25,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Test Cases'!$A$1:$E$71</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1:N14"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="321">
   <si>
     <t>TCID</t>
   </si>
@@ -994,13 +995,15 @@
   </si>
   <si>
     <t>FAIL</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -1438,17 +1441,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="39.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="87.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="6.8046875" collapsed="true"/>
+    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="87.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="16" customFormat="1">
@@ -2997,7 +3000,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -3005,8 +3008,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="56.0" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="56" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3041,6 +3044,11 @@
       </c>
       <c r="E2" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="5:5">
+      <c r="E38" t="s">
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -3059,11 +3067,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="55.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="43.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="55" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="43.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3122,10 +3130,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="24.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="24.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3241,9 +3249,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="65.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="1" max="1" width="65.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3317,10 +3325,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="45.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="83.5703125" collapsed="true"/>
-    <col min="4" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3358,12 +3366,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3425,11 +3433,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="70.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="47.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="70.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="47.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3482,17 +3490,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView zoomScale="90" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="70.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="47.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="70.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="47.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3516,8 +3524,8 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75">
-      <c r="A2" s="10">
-        <v>1</v>
+      <c r="A2" s="10" t="s">
+        <v>320</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>20</v>
@@ -3551,10 +3559,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="54.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="11" customFormat="1">
@@ -3671,10 +3679,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="51.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="61.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="61.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3740,17 +3748,17 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A1:D7"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="59.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="59.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3769,7 +3777,7 @@
     </row>
     <row r="2" spans="1:4" ht="15.75">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>25</v>
@@ -3781,37 +3789,37 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75">
-      <c r="A3" s="14" t="s">
-        <v>26</v>
+    <row r="3" spans="1:4" customFormat="1" ht="15.75">
+      <c r="A3" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75">
+    <row r="4" spans="1:4" customFormat="1" ht="15.75">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75">
-      <c r="A5" s="1" t="s">
-        <v>29</v>
+    <row r="5" spans="1:4" customFormat="1" ht="15.75">
+      <c r="A5" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>25</v>
@@ -3823,9 +3831,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75">
+    <row r="6" spans="1:4" customFormat="1" ht="15.75">
       <c r="A6" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>25</v>
@@ -3837,17 +3845,31 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75">
-      <c r="A7" s="8" t="s">
-        <v>31</v>
+    <row r="7" spans="1:4" customFormat="1" ht="15.75">
+      <c r="A7" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" customFormat="1" ht="15.75">
+      <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3866,10 +3888,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="35.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="1" max="1" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="35.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>

<commit_message>
Authoring testscript bug fix
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Authoring.xlsx
+++ b/src/test/resources/xls/Authoring.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="18330" windowHeight="4290" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="17430" windowHeight="2790" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Test Cases'!$A$1:$E$71</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1:N14"/>
+  <oleSize ref="A1:N8"/>
 </workbook>
 </file>
 
@@ -3553,8 +3553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3594,13 +3594,13 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75">
-      <c r="A3" s="14" t="s">
-        <v>26</v>
+      <c r="A3" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -3750,7 +3750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+    <sheetView zoomScale="90" workbookViewId="0">
       <selection activeCell="A8" sqref="A8:D8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adding 1 script in authoring
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Authoring.xlsx
+++ b/src/test/resources/xls/Authoring.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="17430" windowHeight="3990" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="17430" windowHeight="2865"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Test Cases'!$A$1:$E$71</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1:H13"/>
+  <oleSize ref="A1:E8"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="324">
   <si>
     <t>TCID</t>
   </si>
@@ -998,6 +998,15 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Authoring89</t>
+  </si>
+  <si>
+    <t>OPQA-4712</t>
+  </si>
+  <si>
+    <t>Verify that the user is able to add videos for the post</t>
   </si>
 </sst>
 </file>
@@ -1439,10 +1448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E89"/>
+  <dimension ref="A1:E90"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2932,6 +2941,21 @@
         <v>3</v>
       </c>
       <c r="E89" s="1"/>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="D90" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E90" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2992,9 +3016,10 @@
     <hyperlink ref="B86" r:id="rId55" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1203"/>
     <hyperlink ref="B85" r:id="rId56" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1202"/>
     <hyperlink ref="B87" r:id="rId57" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1207"/>
+    <hyperlink ref="B90" r:id="rId58" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4712"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId58"/>
+  <pageSetup orientation="portrait" r:id="rId59"/>
 </worksheet>
 </file>
 
@@ -3431,7 +3456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+    <sheetView zoomScale="90" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adding Authoring Testscript 91
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Authoring.xlsx
+++ b/src/test/resources/xls/Authoring.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="17430" windowHeight="2865"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14520" windowHeight="3210"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="326">
   <si>
     <t>TCID</t>
   </si>
@@ -1007,6 +1007,12 @@
   </si>
   <si>
     <t>Verify that the user is able to add videos for the post</t>
+  </si>
+  <si>
+    <t>Authoring90</t>
+  </si>
+  <si>
+    <t>Authoring91</t>
   </si>
 </sst>
 </file>
@@ -1448,10 +1454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E90"/>
+  <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2956,6 +2962,36 @@
         <v>3</v>
       </c>
       <c r="E90" s="1"/>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="D91" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E91" s="1"/>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B92" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="D92" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E92" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3017,9 +3053,11 @@
     <hyperlink ref="B85" r:id="rId56" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1202"/>
     <hyperlink ref="B87" r:id="rId57" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1207"/>
     <hyperlink ref="B90" r:id="rId58" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4712"/>
+    <hyperlink ref="B91" r:id="rId59" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4712"/>
+    <hyperlink ref="B92" r:id="rId60" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4712"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId59"/>
+  <pageSetup orientation="portrait" r:id="rId61"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Adding Authoring testscript 92
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Authoring.xlsx
+++ b/src/test/resources/xls/Authoring.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="333">
   <si>
     <t>TCID</t>
   </si>
@@ -1013,6 +1013,28 @@
   </si>
   <si>
     <t>Authoring91</t>
+  </si>
+  <si>
+    <t>OPQA-4713</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify that the user is able to remove the video </t>
+  </si>
+  <si>
+    <t>OPQA-4715||OPQA-4716</t>
+  </si>
+  <si>
+    <t>1.Verify that you can only upload videos from youtube,vmvideos(atleast) links
+2.Verify that after adding the video user is able to add post content(text) to it.</t>
+  </si>
+  <si>
+    <t>Authoring92</t>
+  </si>
+  <si>
+    <t>OPQA-5097</t>
+  </si>
+  <si>
+    <t>verify that without text and the title user is not able to post the video.</t>
   </si>
 </sst>
 </file>
@@ -1123,7 +1145,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1159,6 +1181,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1454,10 +1479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E92"/>
+  <dimension ref="A1:E93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H93" sqref="H93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2933,14 +2958,14 @@
       </c>
       <c r="E88" s="1"/>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" ht="45">
       <c r="A89" s="1" t="s">
         <v>295</v>
       </c>
       <c r="B89" s="8" t="s">
         <v>316</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C89" s="4" t="s">
         <v>296</v>
       </c>
       <c r="D89" s="18" t="s">
@@ -2968,30 +2993,45 @@
         <v>324</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="D91" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E91" s="1"/>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" ht="30">
       <c r="A92" s="1" t="s">
         <v>325</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="D92" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E92" s="1"/>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C93" s="20" t="s">
+        <v>332</v>
+      </c>
+      <c r="D93" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E93" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3793,7 +3833,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:4" customFormat="1" ht="15.75">
+    <row r="3" spans="1:4" ht="15.75">
       <c r="A3" s="8" t="s">
         <v>30</v>
       </c>
@@ -3807,7 +3847,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:4" customFormat="1" ht="15.75">
+    <row r="4" spans="1:4" ht="15.75">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
@@ -3821,7 +3861,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" customFormat="1" ht="15.75">
+    <row r="5" spans="1:4" ht="15.75">
       <c r="A5" s="8" t="s">
         <v>30</v>
       </c>
@@ -3835,7 +3875,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:4" customFormat="1" ht="15.75">
+    <row r="6" spans="1:4" ht="15.75">
       <c r="A6" s="8" t="s">
         <v>31</v>
       </c>
@@ -3849,7 +3889,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:4" customFormat="1" ht="15.75">
+    <row r="7" spans="1:4" ht="15.75">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -3863,7 +3903,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:4" customFormat="1" ht="15.75">
+    <row r="8" spans="1:4" ht="15.75">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
Adding Authoring testscript 93
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Authoring.xlsx
+++ b/src/test/resources/xls/Authoring.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="336">
   <si>
     <t>TCID</t>
   </si>
@@ -1035,6 +1035,15 @@
   </si>
   <si>
     <t>verify that without text and the title user is not able to post the video.</t>
+  </si>
+  <si>
+    <t>Authoring93</t>
+  </si>
+  <si>
+    <t>OPQA-4717</t>
+  </si>
+  <si>
+    <t>verify that even while editing the post User can able to add the videos</t>
   </si>
 </sst>
 </file>
@@ -1479,10 +1488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E93"/>
+  <dimension ref="A1:E94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H93" sqref="H93"/>
+    <sheetView tabSelected="1" topLeftCell="D91" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E94" sqref="A1:E94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3032,6 +3041,21 @@
         <v>3</v>
       </c>
       <c r="E93" s="1"/>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="C94" s="20" t="s">
+        <v>335</v>
+      </c>
+      <c r="D94" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E94" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adding Authoring testscript 94
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Authoring.xlsx
+++ b/src/test/resources/xls/Authoring.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="338">
   <si>
     <t>TCID</t>
   </si>
@@ -1044,6 +1044,12 @@
   </si>
   <si>
     <t>verify that even while editing the post User can able to add the videos</t>
+  </si>
+  <si>
+    <t>Authoring94</t>
+  </si>
+  <si>
+    <t>verify that with the use of Quick insert image upload link, user can upload images at any part in post.</t>
   </si>
 </sst>
 </file>
@@ -1488,10 +1494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E94"/>
+  <dimension ref="A1:E95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D91" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E94" sqref="A1:E94"/>
+    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3056,6 +3062,20 @@
         <v>3</v>
       </c>
       <c r="E94" s="1"/>
+    </row>
+    <row r="95" spans="1:5" ht="30">
+      <c r="A95" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="C95" s="20" t="s">
+        <v>337</v>
+      </c>
+      <c r="D95" s="18" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Fix for failing Authoring testscripts
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Authoring.xlsx
+++ b/src/test/resources/xls/Authoring.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="14520" windowHeight="3210"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14520" windowHeight="3975" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Test Cases'!$A$1:$E$71</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1:E8"/>
+  <oleSize ref="A1:F13"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="338">
   <si>
     <t>TCID</t>
   </si>
@@ -1056,6 +1056,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -1496,17 +1497,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="87.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="39.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="87.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="6.8046875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="16" customFormat="1">
@@ -3149,17 +3150,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="55" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="43.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="55.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="43.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3193,7 +3194,7 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>10010</v>
+        <v>20010</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
@@ -3218,10 +3219,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="26.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3337,9 +3338,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="65.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="65.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3413,12 +3414,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="67" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="67.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="47.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3476,10 +3477,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="45.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="83.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="45.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="83.5703125" collapsed="true"/>
+    <col min="4" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3517,12 +3518,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3584,11 +3585,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="70.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="47.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="70.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="47.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3647,10 +3648,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="54.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="11" customFormat="1">
@@ -3767,10 +3768,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="61.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="51.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="61.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3844,9 +3845,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="59.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="59.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3976,10 +3977,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="35.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="35.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -4053,8 +4054,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="56" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="56.0" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">

</xml_diff>

<commit_message>
Multiple files in multiple packages edited to accomodate the Authoring common Method relocation
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Authoring.xlsx
+++ b/src/test/resources/xls/Authoring.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="338">
   <si>
     <t>TCID</t>
   </si>
@@ -1055,6 +1055,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -1509,11 +1510,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="87.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="39.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="87.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="6.8046875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="16" customFormat="1">
@@ -3162,11 +3163,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="55" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="43.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="55.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="43.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3225,10 +3226,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="26.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3344,9 +3345,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="65.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="65.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3420,12 +3421,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="67" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="47.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="67.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="47.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3483,10 +3484,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="45.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="83.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="45.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="83.5703125" collapsed="true"/>
+    <col min="4" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3524,12 +3525,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3591,11 +3592,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="70.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="47.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="70.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="47.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3654,10 +3655,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="54.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="11" customFormat="1">
@@ -3774,10 +3775,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="61.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="51.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="61.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3851,9 +3852,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="59.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="59.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3983,10 +3984,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="35.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="35.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -4060,7 +4061,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="57.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="57.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">

</xml_diff>

<commit_message>
Fix for branding changes in url
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Authoring.xlsx
+++ b/src/test/resources/xls/Authoring.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14520" windowHeight="3105"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15495" windowHeight="2610" firstSheet="7" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,13 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Test Cases'!$A$1:$E$71</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <oleSize ref="A1:R27"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="338">
   <si>
     <t>TCID</t>
   </si>
@@ -857,19 +858,10 @@
     <t>recordType</t>
   </si>
   <si>
-    <t>/#/wos/491710049WOS1</t>
-  </si>
-  <si>
     <t>ARTICLE</t>
   </si>
   <si>
-    <t>/#/posts/8b28ac5a-db05-4a0d-8da9-3553ebbcd3f2</t>
-  </si>
-  <si>
     <t>POST</t>
-  </si>
-  <si>
-    <t>/#/patents/US20070269858A120071122</t>
   </si>
   <si>
     <t>PATENT</t>
@@ -1049,14 +1041,22 @@
   </si>
   <si>
     <t>OPQA-4719</t>
+  </si>
+  <si>
+    <t>/cmty/#/wos/491710049WOS1</t>
+  </si>
+  <si>
+    <t>/cmty/#/posts/8b28ac5a-db05-4a0d-8da9-3553ebbcd3f2</t>
+  </si>
+  <si>
+    <t>/cmty/#/patents/US20070269858A120071122</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1204,8 +1204,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1260,7 +1288,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1292,9 +1320,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1326,6 +1355,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1501,23 +1531,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A77" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="39.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="87.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="6.8046875" collapsed="true"/>
+    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="87.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="16" customFormat="1">
+    <row r="1" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -1534,12 +1564,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>233</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>37</v>
@@ -1551,12 +1581,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>234</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>47</v>
@@ -1568,12 +1598,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>235</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>48</v>
@@ -1585,7 +1615,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>236</v>
       </c>
@@ -1602,7 +1632,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>237</v>
       </c>
@@ -1619,7 +1649,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>238</v>
       </c>
@@ -1636,7 +1666,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>239</v>
       </c>
@@ -1653,7 +1683,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="25.5">
+    <row r="9" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>240</v>
       </c>
@@ -1670,7 +1700,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>241</v>
       </c>
@@ -1687,7 +1717,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>172</v>
       </c>
@@ -1704,7 +1734,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>173</v>
       </c>
@@ -1721,7 +1751,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>174</v>
       </c>
@@ -1738,7 +1768,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>175</v>
       </c>
@@ -1755,7 +1785,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>176</v>
       </c>
@@ -1772,7 +1802,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>177</v>
       </c>
@@ -1789,12 +1819,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>178</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>68</v>
@@ -1806,7 +1836,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>179</v>
       </c>
@@ -1823,7 +1853,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>180</v>
       </c>
@@ -1840,7 +1870,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>181</v>
       </c>
@@ -1857,7 +1887,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
         <v>182</v>
       </c>
@@ -1874,7 +1904,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
         <v>183</v>
       </c>
@@ -1891,12 +1921,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
         <v>184</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C23" s="18" t="s">
         <v>73</v>
@@ -1908,7 +1938,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
         <v>185</v>
       </c>
@@ -1925,7 +1955,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
         <v>186</v>
       </c>
@@ -1942,7 +1972,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
         <v>187</v>
       </c>
@@ -1959,7 +1989,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
         <v>188</v>
       </c>
@@ -1976,7 +2006,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
         <v>189</v>
       </c>
@@ -1993,7 +2023,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="25.5">
+    <row r="29" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
         <v>190</v>
       </c>
@@ -2010,12 +2040,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
         <v>191</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>85</v>
@@ -2027,7 +2057,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="25.5">
+    <row r="31" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
         <v>192</v>
       </c>
@@ -2044,7 +2074,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="25.5">
+    <row r="32" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
         <v>193</v>
       </c>
@@ -2061,12 +2091,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
         <v>194</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C33" s="18" t="s">
         <v>88</v>
@@ -2078,7 +2108,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
         <v>195</v>
       </c>
@@ -2095,7 +2125,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
         <v>196</v>
       </c>
@@ -2112,7 +2142,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
         <v>197</v>
       </c>
@@ -2129,7 +2159,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
         <v>198</v>
       </c>
@@ -2146,7 +2176,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="25.5">
+    <row r="38" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
         <v>199</v>
       </c>
@@ -2163,7 +2193,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="25.5">
+    <row r="39" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A39" s="18" t="s">
         <v>200</v>
       </c>
@@ -2180,12 +2210,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
         <v>201</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C40" s="18" t="s">
         <v>93</v>
@@ -2197,12 +2227,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="18" t="s">
         <v>202</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C41" s="18" t="s">
         <v>94</v>
@@ -2214,7 +2244,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
         <v>203</v>
       </c>
@@ -2231,7 +2261,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
         <v>204</v>
       </c>
@@ -2248,7 +2278,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
         <v>205</v>
       </c>
@@ -2265,7 +2295,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="18" t="s">
         <v>206</v>
       </c>
@@ -2282,7 +2312,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="18" t="s">
         <v>207</v>
       </c>
@@ -2299,7 +2329,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="18" t="s">
         <v>208</v>
       </c>
@@ -2316,12 +2346,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="18" t="s">
         <v>209</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>131</v>
@@ -2333,12 +2363,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="18" t="s">
         <v>210</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>132</v>
@@ -2350,7 +2380,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
         <v>211</v>
       </c>
@@ -2367,12 +2397,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="18" t="s">
         <v>212</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>135</v>
@@ -2384,12 +2414,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="18" t="s">
         <v>213</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>136</v>
@@ -2401,7 +2431,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="18" t="s">
         <v>214</v>
       </c>
@@ -2418,7 +2448,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="18" t="s">
         <v>215</v>
       </c>
@@ -2435,7 +2465,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="18" t="s">
         <v>216</v>
       </c>
@@ -2452,7 +2482,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="18" t="s">
         <v>217</v>
       </c>
@@ -2469,7 +2499,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="18" t="s">
         <v>218</v>
       </c>
@@ -2486,7 +2516,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="18" t="s">
         <v>219</v>
       </c>
@@ -2503,12 +2533,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="18" t="s">
         <v>220</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C59" s="8" t="s">
         <v>149</v>
@@ -2520,7 +2550,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="18" t="s">
         <v>221</v>
       </c>
@@ -2537,7 +2567,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="18" t="s">
         <v>222</v>
       </c>
@@ -2554,7 +2584,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="18" t="s">
         <v>223</v>
       </c>
@@ -2571,7 +2601,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="18" t="s">
         <v>224</v>
       </c>
@@ -2582,13 +2612,13 @@
         <v>157</v>
       </c>
       <c r="D63" s="18" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="30">
+    <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="18" t="s">
         <v>225</v>
       </c>
@@ -2605,12 +2635,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="18" t="s">
         <v>226</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>160</v>
@@ -2622,7 +2652,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="18" t="s">
         <v>227</v>
       </c>
@@ -2639,7 +2669,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="18" t="s">
         <v>228</v>
       </c>
@@ -2656,7 +2686,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="18" t="s">
         <v>229</v>
       </c>
@@ -2673,7 +2703,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="30">
+    <row r="69" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="18" t="s">
         <v>230</v>
       </c>
@@ -2690,7 +2720,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="18" t="s">
         <v>231</v>
       </c>
@@ -2707,7 +2737,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="18" t="s">
         <v>232</v>
       </c>
@@ -2724,12 +2754,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="18" t="s">
         <v>242</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>245</v>
@@ -2741,7 +2771,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="18" t="s">
         <v>243</v>
       </c>
@@ -2756,7 +2786,7 @@
       </c>
       <c r="E73" s="1"/>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="18" t="s">
         <v>244</v>
       </c>
@@ -2771,7 +2801,7 @@
       </c>
       <c r="E74" s="1"/>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>248</v>
       </c>
@@ -2786,12 +2816,12 @@
       </c>
       <c r="E75" s="1"/>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>251</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>253</v>
@@ -2801,12 +2831,12 @@
       </c>
       <c r="E76" s="1"/>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>252</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>254</v>
@@ -2816,12 +2846,12 @@
       </c>
       <c r="E77" s="1"/>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>256</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C78" s="8" t="s">
         <v>257</v>
@@ -2831,12 +2861,12 @@
       </c>
       <c r="E78" s="1"/>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>258</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C79" s="8" t="s">
         <v>259</v>
@@ -2846,7 +2876,7 @@
       </c>
       <c r="E79" s="1"/>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>260</v>
       </c>
@@ -2861,7 +2891,7 @@
       </c>
       <c r="E80" s="1"/>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>263</v>
       </c>
@@ -2876,7 +2906,7 @@
       </c>
       <c r="E81" s="1"/>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>266</v>
       </c>
@@ -2891,7 +2921,7 @@
       </c>
       <c r="E82" s="1"/>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>269</v>
       </c>
@@ -2906,180 +2936,180 @@
       </c>
       <c r="E83" s="1"/>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D84" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E84" s="1"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B84" s="8" t="s">
+      <c r="B85" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D85" s="18" t="s">
+        <v>316</v>
+      </c>
+      <c r="E85" s="1"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B86" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C86" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="D84" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E84" s="1"/>
-    </row>
-    <row r="85" spans="1:5">
-      <c r="A85" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="B85" s="8" t="s">
+      <c r="D86" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E86" s="1"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B87" s="8" t="s">
         <v>287</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C87" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="D85" s="18" t="s">
+      <c r="D87" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E87" s="1"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D88" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E88" s="1"/>
+    </row>
+    <row r="89" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="D89" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E89" s="1"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="C90" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="E85" s="1"/>
-    </row>
-    <row r="86" spans="1:5">
-      <c r="A86" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="B86" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D86" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E86" s="1"/>
-    </row>
-    <row r="87" spans="1:5">
-      <c r="A87" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="B87" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="D87" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E87" s="1"/>
-    </row>
-    <row r="88" spans="1:5">
-      <c r="A88" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="B88" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="D88" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E88" s="1"/>
-    </row>
-    <row r="89" spans="1:5" ht="45">
-      <c r="A89" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="B89" s="8" t="s">
-        <v>316</v>
-      </c>
-      <c r="C89" s="4" t="s">
-        <v>296</v>
-      </c>
-      <c r="D89" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E89" s="1"/>
-    </row>
-    <row r="90" spans="1:5">
-      <c r="A90" s="1" t="s">
+      <c r="D90" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E90" s="1"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="B90" s="8" t="s">
+      <c r="B91" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="D91" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E91" s="1"/>
+    </row>
+    <row r="92" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="C90" s="4" t="s">
-        <v>322</v>
-      </c>
-      <c r="D90" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E90" s="1"/>
-    </row>
-    <row r="91" spans="1:5">
-      <c r="A91" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="B91" s="8" t="s">
+      <c r="B92" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="C92" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="C91" s="4" t="s">
+      <c r="D92" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E92" s="1"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="D91" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E91" s="1"/>
-    </row>
-    <row r="92" spans="1:5" ht="30">
-      <c r="A92" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="B92" s="8" t="s">
+      <c r="B93" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="C92" s="4" t="s">
+      <c r="C93" s="20" t="s">
         <v>328</v>
       </c>
-      <c r="D92" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E92" s="1"/>
-    </row>
-    <row r="93" spans="1:5">
-      <c r="A93" s="1" t="s">
+      <c r="D93" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E93" s="1"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B94" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="C93" s="20" t="s">
+      <c r="C94" s="20" t="s">
         <v>331</v>
       </c>
-      <c r="D93" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E93" s="1"/>
-    </row>
-    <row r="94" spans="1:5">
-      <c r="A94" s="1" t="s">
+      <c r="D94" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E94" s="1"/>
+    </row>
+    <row r="95" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B95" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="C95" s="20" t="s">
         <v>333</v>
-      </c>
-      <c r="C94" s="20" t="s">
-        <v>334</v>
-      </c>
-      <c r="D94" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E94" s="1"/>
-    </row>
-    <row r="95" spans="1:5" ht="30">
-      <c r="A95" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="C95" s="20" t="s">
-        <v>336</v>
       </c>
       <c r="D95" s="18" t="s">
         <v>3</v>
@@ -3154,23 +3184,23 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView zoomScale="90" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="55.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="43.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="55" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="43.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>40</v>
       </c>
@@ -3190,7 +3220,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -3217,22 +3247,22 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView zoomScale="90" workbookViewId="0">
       <selection sqref="A1:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="24.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="24.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>22</v>
       </c>
@@ -3246,7 +3276,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75">
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -3260,7 +3290,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75">
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>26</v>
       </c>
@@ -3274,7 +3304,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75">
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -3288,7 +3318,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75">
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
@@ -3302,7 +3332,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75">
+    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>30</v>
       </c>
@@ -3316,7 +3346,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75">
+    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>31</v>
       </c>
@@ -3336,21 +3366,21 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D4"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="65.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="1" max="1" width="65.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>272</v>
       </c>
@@ -3364,12 +3394,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B2" t="s">
         <v>274</v>
-      </c>
-      <c r="B2" t="s">
-        <v>275</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -3378,12 +3408,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>276</v>
+        <v>336</v>
       </c>
       <c r="B3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -3392,12 +3422,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>278</v>
+        <v>337</v>
       </c>
       <c r="B4" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -3412,24 +3442,24 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView zoomScale="90" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="67.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="47.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="67" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="47.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -3449,7 +3479,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -3475,22 +3505,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScale="90" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="45.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="83.5703125" collapsed="true"/>
-    <col min="4" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3503,7 +3533,7 @@
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="48" customHeight="1">
+    <row r="2" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -3516,24 +3546,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView zoomScale="90" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
@@ -3556,7 +3586,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -3583,23 +3613,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView zoomScale="90" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="70.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="47.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="70.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="47.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -3619,9 +3649,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75">
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>20</v>
@@ -3646,22 +3676,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView zoomScale="90" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="54.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="11" customFormat="1">
+    <row r="1" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>22</v>
       </c>
@@ -3675,7 +3705,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75">
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -3689,7 +3719,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75">
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>30</v>
       </c>
@@ -3703,7 +3733,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75">
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -3717,7 +3747,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75">
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
@@ -3731,7 +3761,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75">
+    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>30</v>
       </c>
@@ -3745,7 +3775,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75">
+    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>31</v>
       </c>
@@ -3766,22 +3796,22 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="51.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="61.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="61.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>32</v>
       </c>
@@ -3795,9 +3825,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75">
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>35</v>
@@ -3809,7 +3839,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75">
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
@@ -3823,7 +3853,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="45">
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>36</v>
       </c>
@@ -3843,21 +3873,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView zoomScale="90" workbookViewId="0">
       <selection activeCell="A8" sqref="A8:D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="59.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="59.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>22</v>
       </c>
@@ -3871,7 +3901,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75">
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
@@ -3885,7 +3915,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75">
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>30</v>
       </c>
@@ -3899,7 +3929,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75">
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
@@ -3913,7 +3943,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75">
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>30</v>
       </c>
@@ -3927,7 +3957,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75">
+    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>31</v>
       </c>
@@ -3941,7 +3971,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75">
+    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -3955,7 +3985,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75">
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
@@ -3975,22 +4005,22 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScale="90" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="35.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="1" max="1" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="35.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>32</v>
       </c>
@@ -4004,9 +4034,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75">
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>35</v>
@@ -4018,7 +4048,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75">
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
@@ -4032,7 +4062,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="45">
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>36</v>
       </c>
@@ -4052,19 +4082,19 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScale="90" workbookViewId="0">
       <selection activeCell="E2" sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="57.140625" collapsed="true"/>
+    <col min="1" max="1" width="57.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>44</v>
       </c>
@@ -4081,7 +4111,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
Fix for Deep linking failures in Authoring Module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Authoring.xlsx
+++ b/src/test/resources/xls/Authoring.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15495" windowHeight="2610" firstSheet="7" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13935" windowHeight="2580" firstSheet="7" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -1043,13 +1043,13 @@
     <t>OPQA-4719</t>
   </si>
   <si>
-    <t>/cmty/#/wos/491710049WOS1</t>
-  </si>
-  <si>
-    <t>/cmty/#/posts/8b28ac5a-db05-4a0d-8da9-3553ebbcd3f2</t>
-  </si>
-  <si>
-    <t>/cmty/#/patents/US20070269858A120071122</t>
+    <t>cmty/#/wos/491710049WOS1</t>
+  </si>
+  <si>
+    <t>cmty/#/posts/8b28ac5a-db05-4a0d-8da9-3553ebbcd3f2</t>
+  </si>
+  <si>
+    <t>cmty/#/patents/US20070269858A120071122</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Failing Authoring testscript fix
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Authoring.xlsx
+++ b/src/test/resources/xls/Authoring.xlsx
@@ -24,7 +24,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Test Cases'!$A$1:$E$71</definedName>
   </definedNames>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <oleSize ref="A1:R27"/>
 </workbook>
 </file>
@@ -1043,13 +1043,13 @@
     <t>OPQA-4719</t>
   </si>
   <si>
-    <t>cmty/#/wos/491710049WOS1</t>
-  </si>
-  <si>
-    <t>cmty/#/posts/8b28ac5a-db05-4a0d-8da9-3553ebbcd3f2</t>
-  </si>
-  <si>
-    <t>cmty/#/patents/US20070269858A120071122</t>
+    <t>/cmty/#/wos/491710049WOS1</t>
+  </si>
+  <si>
+    <t>/cmty/#/posts/8b28ac5a-db05-4a0d-8da9-3553ebbcd3f2</t>
+  </si>
+  <si>
+    <t>/cmty/#/patents/US20070269858A120071122</t>
   </si>
 </sst>
 </file>

</xml_diff>